<commit_message>
IRPP sources data modification
</commit_message>
<xml_diff>
--- a/src/countries/france/data/sources/IRPP_PPE.xlsx
+++ b/src/countries/france/data/sources/IRPP_PPE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="7395" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="18900" windowHeight="12945" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="benef" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="sources" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <oleSize ref="A1:N41"/>
 </workbook>
 </file>
 
@@ -173,11 +174,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="#,##0&quot;  &quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0\ _€"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0&quot;  &quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0\ _€"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -929,15 +930,15 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -947,113 +948,113 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1075,49 +1076,49 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="6" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1126,28 +1127,25 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1157,26 +1155,29 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1484,7 +1485,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,39 +1495,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="138">
+      <c r="B1" s="137">
         <v>2002</v>
       </c>
-      <c r="C1" s="137">
+      <c r="C1" s="136">
         <v>2003</v>
       </c>
-      <c r="D1" s="137">
+      <c r="D1" s="136">
         <v>2004</v>
       </c>
-      <c r="E1" s="137">
+      <c r="E1" s="136">
         <v>2005</v>
       </c>
-      <c r="F1" s="137">
+      <c r="F1" s="136">
         <v>2006</v>
       </c>
-      <c r="G1" s="137">
+      <c r="G1" s="136">
         <v>2007</v>
       </c>
-      <c r="H1" s="137">
+      <c r="H1" s="136">
         <v>2008</v>
       </c>
-      <c r="I1" s="137">
+      <c r="I1" s="136">
         <v>2009</v>
       </c>
-      <c r="J1" s="137">
+      <c r="J1" s="136">
         <v>2010</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="135" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="130"/>
@@ -1554,7 +1555,7 @@
       <c r="J2" s="131"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="135" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="132"/>
@@ -1576,11 +1577,13 @@
       <c r="H3" s="131">
         <v>7984054</v>
       </c>
-      <c r="I3" s="131"/>
+      <c r="I3" s="131">
+        <v>7126463</v>
+      </c>
       <c r="J3" s="131"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="136" t="s">
+      <c r="A4" s="135" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="74"/>
@@ -1594,7 +1597,7 @@
       <c r="J4" s="74"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="136" t="s">
+      <c r="A5" s="135" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="74"/>
@@ -1615,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,76 +1637,72 @@
     <col min="11" max="11" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="141">
+      <c r="B1" s="140">
         <v>2002</v>
       </c>
-      <c r="C1" s="142">
+      <c r="C1" s="141">
         <v>2003</v>
       </c>
-      <c r="D1" s="142">
+      <c r="D1" s="141">
         <v>2004</v>
       </c>
-      <c r="E1" s="142">
+      <c r="E1" s="141">
         <v>2005</v>
       </c>
-      <c r="F1" s="142">
+      <c r="F1" s="141">
         <v>2006</v>
       </c>
-      <c r="G1" s="142">
+      <c r="G1" s="141">
         <v>2007</v>
       </c>
-      <c r="H1" s="142">
+      <c r="H1" s="141">
         <v>2008</v>
       </c>
-      <c r="I1" s="142">
+      <c r="I1" s="141">
         <v>2009</v>
       </c>
-      <c r="J1" s="142">
+      <c r="J1" s="141">
         <v>2010</v>
       </c>
-      <c r="K1" s="136">
+      <c r="K1" s="135">
         <v>2011</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="134">
-        <v>47300000000</v>
-      </c>
-      <c r="C2" s="134">
-        <v>47600000000</v>
-      </c>
-      <c r="D2" s="134">
-        <v>49400000000</v>
-      </c>
-      <c r="E2" s="134">
-        <v>52400000000</v>
-      </c>
-      <c r="F2" s="134">
-        <v>48600000000</v>
-      </c>
-      <c r="G2" s="134">
-        <v>50900000000</v>
-      </c>
-      <c r="H2" s="134">
-        <v>46100000000</v>
-      </c>
-      <c r="I2" s="134">
-        <v>47000000000</v>
-      </c>
-      <c r="J2" s="134">
-        <v>50600000000</v>
-      </c>
-      <c r="K2" s="74"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="136" t="s">
+      <c r="B2" s="140"/>
+      <c r="C2" s="147">
+        <v>46093751436</v>
+      </c>
+      <c r="D2" s="147">
+        <v>48002550259</v>
+      </c>
+      <c r="E2" s="147">
+        <v>49400964913</v>
+      </c>
+      <c r="F2" s="147">
+        <v>45440685347</v>
+      </c>
+      <c r="G2" s="147">
+        <v>48653656043</v>
+      </c>
+      <c r="H2" s="147">
+        <v>44462573979</v>
+      </c>
+      <c r="I2" s="147">
+        <v>45006902661</v>
+      </c>
+      <c r="J2" s="141"/>
+      <c r="K2" s="135"/>
+    </row>
+    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="135" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="132"/>
@@ -1725,15 +1724,17 @@
       <c r="H3" s="134">
         <v>3793069273</v>
       </c>
-      <c r="I3" s="135"/>
+      <c r="I3" s="131">
+        <v>3205371604</v>
+      </c>
       <c r="J3" s="131"/>
       <c r="K3" s="132"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="140" t="s">
+    <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="139" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="139"/>
+      <c r="B4" s="138"/>
       <c r="C4" s="134">
         <v>64100000000</v>
       </c>
@@ -1762,11 +1763,11 @@
         <v>87400000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="140" t="s">
+    <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="139"/>
+      <c r="B5" s="138"/>
       <c r="C5" s="134">
         <v>4800000000</v>
       </c>
@@ -1795,6 +1796,7 @@
         <v>6300000000</v>
       </c>
     </row>
+    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1806,7 +1808,7 @@
   <dimension ref="A1:CG36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:J8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,7 +2474,9 @@
       <c r="H8" s="9">
         <v>7984054</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="9">
+        <v>7126463</v>
+      </c>
       <c r="J8" s="38"/>
       <c r="K8" s="90"/>
       <c r="L8" s="90"/>
@@ -2573,7 +2577,9 @@
       <c r="H9" s="9">
         <v>3481494</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9">
+        <v>3920593</v>
+      </c>
       <c r="J9" s="38"/>
       <c r="K9" s="90"/>
       <c r="L9" s="90"/>
@@ -2674,7 +2680,9 @@
       <c r="H10" s="41">
         <v>4502560</v>
       </c>
-      <c r="I10" s="41"/>
+      <c r="I10" s="41">
+        <v>3205870</v>
+      </c>
       <c r="J10" s="42"/>
       <c r="K10" s="90"/>
       <c r="L10" s="90"/>
@@ -3180,7 +3188,9 @@
       <c r="H15" s="48">
         <v>8208245</v>
       </c>
-      <c r="I15" s="48"/>
+      <c r="I15" s="48">
+        <v>7328830</v>
+      </c>
       <c r="J15" s="61"/>
       <c r="K15" s="90"/>
       <c r="L15" s="90"/>
@@ -3281,7 +3291,9 @@
       <c r="H16" s="9">
         <v>3525382</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="9">
+        <v>4080784</v>
+      </c>
       <c r="J16" s="38"/>
       <c r="K16" s="90"/>
       <c r="L16" s="90"/>
@@ -3382,7 +3394,9 @@
       <c r="H17" s="41">
         <v>4682863</v>
       </c>
-      <c r="I17" s="41"/>
+      <c r="I17" s="41">
+        <v>3248046</v>
+      </c>
       <c r="J17" s="42"/>
       <c r="K17" s="90"/>
       <c r="L17" s="90"/>
@@ -4350,7 +4364,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="C5" sqref="C5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4542,7 +4556,9 @@
       <c r="H7" s="66">
         <v>3793069273</v>
       </c>
-      <c r="I7" s="27"/>
+      <c r="I7" s="27">
+        <v>3205371604</v>
+      </c>
       <c r="J7" s="115"/>
       <c r="K7" s="120"/>
     </row>
@@ -4569,7 +4585,9 @@
       <c r="H8" s="10">
         <v>1533120926</v>
       </c>
-      <c r="I8" s="27"/>
+      <c r="I8" s="27">
+        <v>1852239470</v>
+      </c>
       <c r="J8" s="115"/>
       <c r="K8" s="74"/>
     </row>
@@ -4596,7 +4614,9 @@
       <c r="H9" s="40">
         <v>2259948347</v>
       </c>
-      <c r="I9" s="53"/>
+      <c r="I9" s="53">
+        <v>1353132134</v>
+      </c>
       <c r="J9" s="116"/>
       <c r="K9" s="74"/>
     </row>
@@ -4725,7 +4745,9 @@
       <c r="H14" s="9">
         <v>3917700000</v>
       </c>
-      <c r="I14" s="27"/>
+      <c r="I14" s="27">
+        <v>3311161047</v>
+      </c>
       <c r="J14" s="115"/>
       <c r="K14" s="74"/>
     </row>
@@ -4752,7 +4774,9 @@
       <c r="H15" s="9">
         <v>1553200000</v>
       </c>
-      <c r="I15" s="27"/>
+      <c r="I15" s="27">
+        <v>1939476703</v>
+      </c>
       <c r="J15" s="115"/>
       <c r="K15" s="74"/>
     </row>
@@ -4779,7 +4803,9 @@
       <c r="H16" s="126">
         <v>2364500000</v>
       </c>
-      <c r="I16" s="127"/>
+      <c r="I16" s="127">
+        <v>1371684344</v>
+      </c>
       <c r="J16" s="128"/>
       <c r="K16" s="17"/>
       <c r="L16" s="28"/>
@@ -4788,7 +4814,7 @@
       <c r="A17" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="144"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="107">
         <v>2003</v>
       </c>
@@ -4816,13 +4842,13 @@
       <c r="K17" s="108">
         <v>2011</v>
       </c>
-      <c r="L17" s="147"/>
+      <c r="L17" s="146"/>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="143"/>
+      <c r="B18" s="142"/>
       <c r="C18" s="72">
         <v>64100000000</v>
       </c>
@@ -4850,13 +4876,13 @@
       <c r="K18" s="105">
         <v>87400000000</v>
       </c>
-      <c r="L18" s="147"/>
+      <c r="L18" s="146"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="143"/>
+      <c r="B19" s="142"/>
       <c r="C19" s="72">
         <v>4800000000</v>
       </c>
@@ -4884,7 +4910,7 @@
       <c r="K19" s="105">
         <v>6300000000</v>
       </c>
-      <c r="L19" s="147"/>
+      <c r="L19" s="146"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
@@ -4917,8 +4943,8 @@
       <c r="J20" s="72">
         <v>50600000000</v>
       </c>
-      <c r="K20" s="145"/>
-      <c r="L20" s="147"/>
+      <c r="K20" s="144"/>
+      <c r="L20" s="146"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="104" t="s">
@@ -4951,8 +4977,8 @@
       <c r="J21" s="106">
         <v>41900000000</v>
       </c>
-      <c r="K21" s="146"/>
-      <c r="L21" s="147"/>
+      <c r="K21" s="145"/>
+      <c r="L21" s="146"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L22" s="133"/>

</xml_diff>

<commit_message>
change code fami as famille in param
</commit_message>
<xml_diff>
--- a/src/countries/france/data/sources/IRPP_PPE.xlsx
+++ b/src/countries/france/data/sources/IRPP_PPE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20355" windowHeight="12945" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15960" windowHeight="10665" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="benef" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="sources" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <oleSize ref="A1:J41"/>
+  <oleSize ref="C1:J9"/>
 </workbook>
 </file>
 
@@ -1492,7 +1492,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection sqref="A1:K5"/>
     </sheetView>
   </sheetViews>
@@ -1817,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J18"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4387,8 +4387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "api et nouvelles donn?es irpp"
This reverts commit 2e66abfb886296033fd427d0f5fba8a5915827eb.

Conflicts:
	src/countries/france/data/amounts.h5
	src/countries/france/data/sources/IRPP_PPE.xlsx
	src/scripts/aggregates_all_years.py
</commit_message>
<xml_diff>
--- a/src/countries/france/data/sources/IRPP_PPE.xlsx
+++ b/src/countries/france/data/sources/IRPP_PPE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15960" windowHeight="10665" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14640" windowHeight="12945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="benef" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="sources" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <oleSize ref="C1:J9"/>
+  <oleSize ref="D10:K50"/>
 </workbook>
 </file>
 
@@ -180,7 +180,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,12 +300,6 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1180,12 +1174,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers" xfId="2" builtinId="3"/>
@@ -1492,7 +1486,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1701,7 @@
       <c r="I2" s="143">
         <v>45006902661</v>
       </c>
-      <c r="J2" s="147">
+      <c r="J2" s="146">
         <v>48718114427</v>
       </c>
       <c r="K2" s="132"/>
@@ -1817,7 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG36"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -4387,8 +4381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4688,7 +4682,9 @@
       <c r="H11" s="56">
         <v>48435000000</v>
       </c>
-      <c r="I11" s="145"/>
+      <c r="I11" s="148">
+        <v>48558550123</v>
+      </c>
       <c r="J11" s="116"/>
       <c r="K11" s="72"/>
     </row>
@@ -4718,7 +4714,7 @@
       <c r="I12" s="53">
         <v>45469619577</v>
       </c>
-      <c r="J12" s="146">
+      <c r="J12" s="145">
         <v>49218114427</v>
       </c>
       <c r="K12" s="72"/>
@@ -4874,7 +4870,7 @@
       <c r="K17" s="106">
         <v>2011</v>
       </c>
-      <c r="L17" s="148"/>
+      <c r="L17" s="147"/>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="101" t="s">
@@ -4908,7 +4904,7 @@
       <c r="K18" s="103">
         <v>87400000000</v>
       </c>
-      <c r="L18" s="148"/>
+      <c r="L18" s="147"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="101" t="s">
@@ -4942,7 +4938,7 @@
       <c r="K19" s="103">
         <v>6300000000</v>
       </c>
-      <c r="L19" s="148"/>
+      <c r="L19" s="147"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
@@ -4976,7 +4972,7 @@
         <v>50600000000</v>
       </c>
       <c r="K20" s="141"/>
-      <c r="L20" s="148"/>
+      <c r="L20" s="147"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="102" t="s">
@@ -5010,7 +5006,7 @@
         <v>41900000000</v>
       </c>
       <c r="K21" s="142"/>
-      <c r="L21" s="148"/>
+      <c r="L21" s="147"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L22" s="130"/>

</xml_diff>

<commit_message>
Revert "Revert "api et nouvelles donn?es irpp""
This reverts commit b74052a436710b3b0e8e27df84b628d9ebfc7e1c.
</commit_message>
<xml_diff>
--- a/src/countries/france/data/sources/IRPP_PPE.xlsx
+++ b/src/countries/france/data/sources/IRPP_PPE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14640" windowHeight="12945" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15960" windowHeight="10665" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="benef" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="sources" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <oleSize ref="D10:K50"/>
+  <oleSize ref="C1:J9"/>
 </workbook>
 </file>
 
@@ -180,7 +180,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +300,12 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1174,12 +1180,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers" xfId="2" builtinId="3"/>
@@ -1486,7 +1492,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,7 +1707,7 @@
       <c r="I2" s="143">
         <v>45006902661</v>
       </c>
-      <c r="J2" s="146">
+      <c r="J2" s="147">
         <v>48718114427</v>
       </c>
       <c r="K2" s="132"/>
@@ -1811,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -4381,8 +4387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4682,9 +4688,7 @@
       <c r="H11" s="56">
         <v>48435000000</v>
       </c>
-      <c r="I11" s="148">
-        <v>48558550123</v>
-      </c>
+      <c r="I11" s="145"/>
       <c r="J11" s="116"/>
       <c r="K11" s="72"/>
     </row>
@@ -4714,7 +4718,7 @@
       <c r="I12" s="53">
         <v>45469619577</v>
       </c>
-      <c r="J12" s="145">
+      <c r="J12" s="146">
         <v>49218114427</v>
       </c>
       <c r="K12" s="72"/>
@@ -4870,7 +4874,7 @@
       <c r="K17" s="106">
         <v>2011</v>
       </c>
-      <c r="L17" s="147"/>
+      <c r="L17" s="148"/>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="101" t="s">
@@ -4904,7 +4908,7 @@
       <c r="K18" s="103">
         <v>87400000000</v>
       </c>
-      <c r="L18" s="147"/>
+      <c r="L18" s="148"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="101" t="s">
@@ -4938,7 +4942,7 @@
       <c r="K19" s="103">
         <v>6300000000</v>
       </c>
-      <c r="L19" s="147"/>
+      <c r="L19" s="148"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
@@ -4972,7 +4976,7 @@
         <v>50600000000</v>
       </c>
       <c r="K20" s="141"/>
-      <c r="L20" s="147"/>
+      <c r="L20" s="148"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="102" t="s">
@@ -5006,7 +5010,7 @@
         <v>41900000000</v>
       </c>
       <c r="K21" s="142"/>
-      <c r="L21" s="147"/>
+      <c r="L21" s="148"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L22" s="130"/>

</xml_diff>